<commit_message>
Deploying to gh-pages from  @ 40b2334697a4304d51e53cc97cc05e6a3988529c 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/17.1.1.xlsx
+++ b/en/downloads/data-excel/17.1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Глобальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Глобальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>(в процентах  к ВВП)</t>
   </si>
@@ -117,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +241,12 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,7 +304,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -397,6 +403,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -679,9 +688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,7 +700,7 @@
     <col min="13" max="15" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
@@ -712,7 +723,7 @@
       <c r="N1" s="26"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
@@ -735,7 +746,7 @@
       <c r="N2" s="3"/>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -752,7 +763,7 @@
       <c r="N3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>18</v>
       </c>
@@ -801,8 +812,11 @@
       <c r="P4" s="14">
         <v>2019</v>
       </c>
+      <c r="Q4" s="14">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>20</v>
       </c>
@@ -851,8 +865,11 @@
       <c r="P5" s="28">
         <v>27</v>
       </c>
+      <c r="Q5" s="38">
+        <v>25.3</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -901,8 +918,11 @@
       <c r="P6" s="31">
         <v>19.600000000000001</v>
       </c>
+      <c r="Q6" s="30">
+        <v>17.8</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
@@ -951,8 +971,11 @@
       <c r="P7" s="31" t="s">
         <v>6</v>
       </c>
+      <c r="Q7" s="30" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>26</v>
       </c>
@@ -1001,8 +1024,11 @@
       <c r="P8" s="31">
         <v>2.2000000000000002</v>
       </c>
+      <c r="Q8" s="30">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -1051,8 +1077,11 @@
       <c r="P9" s="32">
         <v>5.2</v>
       </c>
+      <c r="Q9" s="32">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>22</v>
       </c>
@@ -1101,8 +1130,11 @@
       <c r="P10" s="34">
         <v>0</v>
       </c>
+      <c r="Q10" s="34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="8"/>
       <c r="C11" s="25"/>
@@ -1120,7 +1152,7 @@
       <c r="O11" s="26"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
     </row>
   </sheetData>

</xml_diff>